<commit_message>
shifted conf to Econf.pm. Better this way!
</commit_message>
<xml_diff>
--- a/mybook.xlsx
+++ b/mybook.xlsx
@@ -346,7 +346,12 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -361,7 +366,12 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added new EW2 and 2test.pl. new way!
</commit_message>
<xml_diff>
--- a/mybook.xlsx
+++ b/mybook.xlsx
@@ -366,12 +366,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>